<commit_message>
A Fazer as tabelas
</commit_message>
<xml_diff>
--- a/Versão Final/Tabelas.xlsx
+++ b/Versão Final/Tabelas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Documents\Projectos\Escola\Projecto_RC\Versão Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Projecto_RC\Versão Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="5664" tabRatio="729" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="5670" tabRatio="729" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Distribuição Postos por Salas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="363">
   <si>
     <t>Número Sala</t>
   </si>
@@ -1066,6 +1065,63 @@
   </si>
   <si>
     <t>172.20.35.170</t>
+  </si>
+  <si>
+    <t>SW1.3</t>
+  </si>
+  <si>
+    <t>MUDEI DE SWITCH- 4 portas vagas</t>
+  </si>
+  <si>
+    <t>1.7.5A</t>
+  </si>
+  <si>
+    <t>1.7.5B</t>
+  </si>
+  <si>
+    <t>1.9.4B</t>
+  </si>
+  <si>
+    <t>1.9.3A</t>
+  </si>
+  <si>
+    <t>1.9.3B</t>
+  </si>
+  <si>
+    <t>1.9.4A</t>
+  </si>
+  <si>
+    <t>1.10.3A</t>
+  </si>
+  <si>
+    <t>1.10.3B</t>
+  </si>
+  <si>
+    <t>1.10.4A</t>
+  </si>
+  <si>
+    <t>1.10.4B</t>
+  </si>
+  <si>
+    <t>MUDEI DE SWITCH- 4 portas livres</t>
+  </si>
+  <si>
+    <t>"1.10"</t>
+  </si>
+  <si>
+    <t>1.12.3A</t>
+  </si>
+  <si>
+    <t>1.12.3B</t>
+  </si>
+  <si>
+    <t>1.12.4A</t>
+  </si>
+  <si>
+    <t>1.12.4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTOU AQUI </t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1114,6 +1170,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1127,7 +1195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1172,6 +1240,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3085,21 +3162,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Identificação"/>
-      <sheetName val="Opções"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Tabela"/>
       <sheetName val="Opções"/>
     </sheetNames>
@@ -3187,8 +3249,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="A3:G121" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A3:G121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="A3:G135" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A3:G135"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Sala" dataDxfId="6"/>
     <tableColumn id="2" name="Tomada" dataDxfId="5"/>
@@ -3230,7 +3292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3529,27 +3591,27 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" customWidth="1"/>
-    <col min="5" max="5" width="27.21875" customWidth="1"/>
-    <col min="6" max="6" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3569,7 +3631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -3591,7 +3653,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -3613,7 +3675,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -3635,7 +3697,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -3657,7 +3719,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -3679,7 +3741,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -3701,7 +3763,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -3723,7 +3785,7 @@
       </c>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -3745,7 +3807,7 @@
       </c>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -3767,7 +3829,7 @@
       </c>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -3789,7 +3851,7 @@
       </c>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -3811,7 +3873,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -3833,7 +3895,7 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -3855,7 +3917,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -3877,7 +3939,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -3899,7 +3961,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -3921,7 +3983,7 @@
       </c>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -3943,7 +4005,7 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -3965,7 +4027,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -3986,7 +4048,7 @@
       </c>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -4007,7 +4069,7 @@
       </c>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -4029,22 +4091,22 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>265</v>
       </c>
@@ -4068,20 +4130,20 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>268</v>
       </c>
@@ -4098,7 +4160,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>99</v>
       </c>
@@ -4116,7 +4178,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -4131,7 +4193,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>20</v>
       </c>
@@ -4146,7 +4208,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>30</v>
       </c>
@@ -4161,7 +4223,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>40</v>
       </c>
@@ -4176,7 +4238,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>50</v>
       </c>
@@ -4191,7 +4253,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>60</v>
       </c>
@@ -4206,7 +4268,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>70</v>
       </c>
@@ -4221,7 +4283,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>80</v>
       </c>
@@ -4236,7 +4298,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>90</v>
       </c>
@@ -4251,14 +4313,14 @@
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>267</v>
       </c>
@@ -4287,7 +4349,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>90</v>
       </c>
@@ -4316,7 +4378,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>10</v>
       </c>
@@ -4345,7 +4407,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>99</v>
       </c>
@@ -4368,7 +4430,7 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>20</v>
       </c>
@@ -4391,7 +4453,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>30</v>
       </c>
@@ -4414,7 +4476,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>60</v>
       </c>
@@ -4437,7 +4499,7 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>70</v>
       </c>
@@ -4460,7 +4522,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>40</v>
       </c>
@@ -4483,7 +4545,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>50</v>
       </c>
@@ -4506,7 +4568,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>80</v>
       </c>
@@ -4529,7 +4591,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -4540,7 +4602,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -4551,7 +4613,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -4562,7 +4624,7 @@
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -4573,7 +4635,7 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -4584,7 +4646,7 @@
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>305</v>
       </c>
@@ -4592,12 +4654,12 @@
         <v>309</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>307</v>
       </c>
@@ -4621,29 +4683,29 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="18"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -4675,7 +4737,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>56</v>
       </c>
@@ -4705,7 +4767,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -4735,7 +4797,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>67</v>
       </c>
@@ -4759,7 +4821,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -4783,7 +4845,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
@@ -4807,7 +4869,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -4831,7 +4893,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
@@ -4855,7 +4917,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>78</v>
       </c>
@@ -4879,7 +4941,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -4903,7 +4965,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>262</v>
       </c>
@@ -4911,47 +4973,47 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>260</v>
       </c>
@@ -4970,33 +5032,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N121"/>
+  <dimension ref="A1:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5028,7 +5090,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>93</v>
       </c>
@@ -5042,7 +5104,7 @@
         <v>96</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>97</v>
@@ -5057,7 +5119,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>93</v>
       </c>
@@ -5071,13 +5133,13 @@
         <v>96</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="L5" t="s">
         <v>86</v>
@@ -5086,7 +5148,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>93</v>
       </c>
@@ -5100,13 +5162,13 @@
         <v>96</v>
       </c>
       <c r="E6" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>97</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L6" t="s">
         <v>40</v>
@@ -5115,19 +5177,27 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>106</v>
+      <c r="C7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="20">
+        <v>6</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="L7" t="s">
         <v>33</v>
@@ -5139,7 +5209,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>93</v>
       </c>
@@ -5160,7 +5230,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>93</v>
       </c>
@@ -5184,7 +5254,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>93</v>
       </c>
@@ -5205,7 +5275,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>93</v>
       </c>
@@ -5229,7 +5299,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>119</v>
       </c>
@@ -5243,7 +5313,7 @@
         <v>96</v>
       </c>
       <c r="E12" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>97</v>
@@ -5252,7 +5322,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>119</v>
       </c>
@@ -5266,16 +5336,16 @@
         <v>96</v>
       </c>
       <c r="E13" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>119</v>
       </c>
@@ -5289,31 +5359,39 @@
         <v>96</v>
       </c>
       <c r="E14" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="20">
+        <v>10</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>119</v>
       </c>
@@ -5331,7 +5409,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>119</v>
       </c>
@@ -5352,7 +5430,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>119</v>
       </c>
@@ -5368,7 +5446,7 @@
       </c>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>119</v>
       </c>
@@ -5383,7 +5461,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>131</v>
       </c>
@@ -5397,7 +5475,7 @@
         <v>96</v>
       </c>
       <c r="E20" s="3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>97</v>
@@ -5406,7 +5484,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>131</v>
       </c>
@@ -5420,16 +5498,16 @@
         <v>96</v>
       </c>
       <c r="E21" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>131</v>
       </c>
@@ -5443,42 +5521,46 @@
         <v>96</v>
       </c>
       <c r="E22" s="3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="20">
+        <v>14</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -5486,16 +5568,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -5503,16 +5583,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -5520,16 +5598,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -5537,7 +5613,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>140</v>
       </c>
@@ -5551,7 +5627,7 @@
         <v>96</v>
       </c>
       <c r="E28" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>97</v>
@@ -5560,7 +5636,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>140</v>
       </c>
@@ -5574,16 +5650,16 @@
         <v>96</v>
       </c>
       <c r="E29" s="3">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>140</v>
       </c>
@@ -5597,31 +5673,39 @@
         <v>96</v>
       </c>
       <c r="E30" s="3">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="20">
+        <v>18</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>140</v>
       </c>
@@ -5636,7 +5720,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>140</v>
       </c>
@@ -5651,7 +5735,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>140</v>
       </c>
@@ -5666,7 +5750,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>140</v>
       </c>
@@ -5681,7 +5765,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>149</v>
       </c>
@@ -5695,7 +5779,7 @@
         <v>96</v>
       </c>
       <c r="E36" s="3">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>97</v>
@@ -5704,22 +5788,33 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C37" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="20">
+        <v>20</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>149</v>
       </c>
@@ -5734,7 +5829,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>149</v>
       </c>
@@ -5749,7 +5844,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>154</v>
       </c>
@@ -5763,7 +5858,7 @@
         <v>156</v>
       </c>
       <c r="E40" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>97</v>
@@ -5772,7 +5867,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>154</v>
       </c>
@@ -5786,16 +5881,16 @@
         <v>156</v>
       </c>
       <c r="E41" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>154</v>
       </c>
@@ -5809,31 +5904,39 @@
         <v>156</v>
       </c>
       <c r="E42" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G42" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" s="20">
+        <v>6</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>154</v>
       </c>
@@ -5848,7 +5951,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>154</v>
       </c>
@@ -5863,7 +5966,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>154</v>
       </c>
@@ -5878,7 +5981,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>154</v>
       </c>
@@ -5893,7 +5996,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>164</v>
       </c>
@@ -5907,7 +6010,7 @@
         <v>156</v>
       </c>
       <c r="E48" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>97</v>
@@ -5916,7 +6019,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>164</v>
       </c>
@@ -5930,16 +6033,16 @@
         <v>156</v>
       </c>
       <c r="E49" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>164</v>
       </c>
@@ -5953,61 +6056,85 @@
         <v>156</v>
       </c>
       <c r="E50" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G50" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E51" s="20">
+        <v>10</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G51" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="B52" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="E52" s="19">
+        <v>11</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C53" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" s="20">
+        <v>12</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>164</v>
       </c>
@@ -6022,7 +6149,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>164</v>
       </c>
@@ -6037,126 +6164,134 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="3">
-        <v>14</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="3">
-        <v>15</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="E58" s="3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G58" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E59" s="3">
+        <v>14</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E60" s="3">
+        <v>15</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C61" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E61" s="20">
+        <v>16</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>173</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -6166,12 +6301,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>173</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -6181,134 +6316,137 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E64" s="3">
-        <v>7</v>
-      </c>
-      <c r="F64" s="3" t="s">
+      <c r="E66" s="3">
+        <v>17</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E65" s="3">
-        <v>8</v>
-      </c>
-      <c r="F65" s="3" t="s">
+      <c r="E67" s="3">
+        <v>18</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B68" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B67" s="5" t="s">
+      <c r="C68" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="E68" s="19">
+        <v>19</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G68" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="20">
+        <v>1.9</v>
+      </c>
+      <c r="B69" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E68" s="3">
-        <v>17</v>
-      </c>
-      <c r="F68" s="3" t="s">
+      <c r="D69" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" s="20">
+        <v>20</v>
+      </c>
+      <c r="F69" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="G68" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E69" s="3">
-        <v>18</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G69" s="3" t="s">
+      <c r="G69" s="20" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>187</v>
+      <c r="H69" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>1.9</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>189</v>
+        <v>349</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -6318,12 +6456,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>187</v>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>1.9</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>190</v>
+        <v>350</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -6333,126 +6471,134 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E72" s="3">
-        <v>19</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E73" s="3">
-        <v>20</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>96</v>
+        <v>344</v>
       </c>
       <c r="E74" s="3">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G74" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E75" s="3">
+        <v>4</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="E76" s="19">
+        <v>5</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="E77" s="20">
+        <v>6</v>
+      </c>
+      <c r="F77" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>191</v>
+        <v>357</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>198</v>
+        <v>352</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -6462,12 +6608,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>191</v>
+        <v>357</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>199</v>
+        <v>353</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -6477,97 +6623,97 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C80" s="3" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E80" s="3">
-        <v>22</v>
-      </c>
-      <c r="F80" s="3" t="s">
+      <c r="D82" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E82" s="3">
+        <v>5</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="G82" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C81" s="3" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E81" s="3">
-        <v>23</v>
-      </c>
-      <c r="F81" s="3" t="s">
+      <c r="D83" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E83" s="3">
+        <v>6</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>156</v>
+        <v>344</v>
       </c>
       <c r="E84" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>97</v>
@@ -6576,81 +6722,65 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C85" s="3" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E85" s="3">
-        <v>10</v>
-      </c>
-      <c r="F85" s="3" t="s">
+      <c r="D85" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="E85" s="20">
+        <v>8</v>
+      </c>
+      <c r="F85" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="G85" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E86" s="3">
-        <v>11</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E87" s="3">
-        <v>12</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G87" s="3" t="s">
+      <c r="G85" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -6660,12 +6790,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -6675,157 +6805,152 @@
         <v>106</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E90" s="3">
+        <v>9</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E91" s="3">
+        <v>10</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B92" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="E92" s="19">
+        <v>11</v>
+      </c>
+      <c r="F92" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="20">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="C93" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D93" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="E93" s="20">
+        <v>12</v>
+      </c>
+      <c r="F93" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G93" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H93" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E92" s="3">
-        <v>13</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E93" s="3">
-        <v>14</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E94" s="3">
-        <v>15</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E95" s="3">
-        <v>16</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E96" s="3">
-        <v>17</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="5" t="s">
-        <v>214</v>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>1.1200000000000001</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>220</v>
+        <v>361</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -6835,42 +6960,58 @@
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E98" s="3">
+        <v>9</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E99" s="3">
+        <v>10</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>95</v>
@@ -6879,7 +7020,7 @@
         <v>156</v>
       </c>
       <c r="E100" s="3">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>97</v>
@@ -6888,12 +7029,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>95</v>
@@ -6902,44 +7043,36 @@
         <v>156</v>
       </c>
       <c r="E101" s="3">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E102" s="3">
-        <v>20</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G102" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -6949,12 +7082,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -6964,12 +7097,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -6979,80 +7112,104 @@
         <v>106</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E106" s="3">
+        <v>13</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E107" s="3">
+        <v>14</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="E108" s="3">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E109" s="3">
+        <v>16</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>95</v>
@@ -7061,44 +7218,36 @@
         <v>156</v>
       </c>
       <c r="E110" s="3">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E111" s="3">
-        <v>22</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G111" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -7108,12 +7257,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -7123,12 +7272,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>95</v>
@@ -7137,21 +7286,21 @@
         <v>156</v>
       </c>
       <c r="E114" s="3">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>95</v>
@@ -7160,47 +7309,47 @@
         <v>156</v>
       </c>
       <c r="E115" s="3">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F115" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B116" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C116" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D116" s="9" t="s">
+      <c r="D116" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E116" s="9">
-        <v>25</v>
-      </c>
-      <c r="F116" s="9" t="s">
+      <c r="E116" s="3">
+        <v>20</v>
+      </c>
+      <c r="F116" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G116" s="9" t="s">
-        <v>242</v>
+      <c r="G116" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="H116" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -7210,12 +7359,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -7225,12 +7374,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -7240,12 +7389,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -7255,12 +7404,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
@@ -7270,45 +7419,276 @@
         <v>106</v>
       </c>
     </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E122" s="3">
+        <v>24</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E124" s="3">
+        <v>21</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E125" s="3">
+        <v>22</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E128" s="3">
+        <v>23</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E129" s="3">
+        <v>24</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D130" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E130" s="9">
+        <v>25</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G130" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+      <c r="G133" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+      <c r="G134" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5"/>
+      <c r="G135" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A78"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'C:\Users\artur\Documents\Projectos\Escola\Projecto_RC\Documentação\Tabelas\[Identificação da cablagem horizontal.xlsx]Opções'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G4:G121</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'C:\Users\artur\Documents\Projectos\Escola\Projecto_RC\Documentação\Tabelas\[Identificação da cablagem horizontal.xlsx]Opções'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>A4:A7 A9:A15 A20:A29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'C:\Users\artur\Documents\Projectos\Escola\Projecto_RC\Documentação\Tabelas\[Identificação da cablagem horizontal.xlsx]Opções'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4:D7 D12:D15 D20:D29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'C:\Users\artur\Documents\Projectos\Escola\Projecto_RC\Documentação\Tabelas\[Identificação da cablagem horizontal.xlsx]Opções'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E4:E7 E12:E15 E20:E29</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7320,24 +7700,24 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -7357,7 +7737,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7371,7 +7751,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -7385,7 +7765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>35</v>
       </c>
@@ -7396,7 +7776,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -7407,7 +7787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -7421,7 +7801,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -7435,7 +7815,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>44</v>
       </c>
@@ -7446,7 +7826,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -7494,14 +7874,14 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Tabela da cabelagem horizontal feita
</commit_message>
<xml_diff>
--- a/Versão Final/Tabelas.xlsx
+++ b/Versão Final/Tabelas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Documents\Projectos\Escola\Projecto_RC\Versão Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Projecto_RC\Versão Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="5676" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22740" windowHeight="5670" tabRatio="729" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Distribuição Postos por Salas" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="402">
   <si>
     <t>Número Sala</t>
   </si>
@@ -673,9 +673,6 @@
     <t>1.13.4A</t>
   </si>
   <si>
-    <t>1.134B</t>
-  </si>
-  <si>
     <t>1.14</t>
   </si>
   <si>
@@ -767,9 +764,6 @@
   </si>
   <si>
     <t>1.20.2A</t>
-  </si>
-  <si>
-    <t>NÃO EXISTE PORTA 25 NO MODELO QUE ESTAMOS A USAR, LOGO OS SWITCHES A USAR NÃO CHEGAM!</t>
   </si>
   <si>
     <t>1.20.2B</t>
@@ -1037,9 +1031,6 @@
     <t>1.12.4B</t>
   </si>
   <si>
-    <t xml:space="preserve">ESTOU AQUI </t>
-  </si>
-  <si>
     <t>172.20.35.128 /28</t>
   </si>
   <si>
@@ -1161,6 +1152,93 @@
   </si>
   <si>
     <t>guest</t>
+  </si>
+  <si>
+    <t>1.13.5A</t>
+  </si>
+  <si>
+    <t>1.13.5B</t>
+  </si>
+  <si>
+    <t>1.13.4B</t>
+  </si>
+  <si>
+    <t>1.14.5A</t>
+  </si>
+  <si>
+    <t>1.14.5B</t>
+  </si>
+  <si>
+    <t>SW1.4</t>
+  </si>
+  <si>
+    <t>SW.14</t>
+  </si>
+  <si>
+    <t>MUDEI DE SWITCH</t>
+  </si>
+  <si>
+    <t>NÃO É SUPOSTO MUDARMOS A SALA DO BASTIDOR ? ESTA AQUI COMO SALA 1.16 MAS OS BASTIDORES ESTÃO NOUTRA SALA AGORA, E TEMOS DOIS BASTIDORES</t>
+  </si>
+  <si>
+    <t>1.16.1A</t>
+  </si>
+  <si>
+    <t>1.16.1B</t>
+  </si>
+  <si>
+    <t>1.16.2A</t>
+  </si>
+  <si>
+    <t>1.16.2B</t>
+  </si>
+  <si>
+    <t>1.17.2A</t>
+  </si>
+  <si>
+    <t>1.17.2B</t>
+  </si>
+  <si>
+    <t>1.17.3A</t>
+  </si>
+  <si>
+    <t>1.17.3B</t>
+  </si>
+  <si>
+    <t>1.17.4A</t>
+  </si>
+  <si>
+    <t>1.17.4B</t>
+  </si>
+  <si>
+    <t>1.17.5A</t>
+  </si>
+  <si>
+    <t>1.17.5B</t>
+  </si>
+  <si>
+    <t>1.17.6A</t>
+  </si>
+  <si>
+    <t>1.17.6B</t>
+  </si>
+  <si>
+    <t>SW1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUDEI DE SWITCH </t>
+  </si>
+  <si>
+    <t>1.18.3A</t>
+  </si>
+  <si>
+    <t>1.18.3B</t>
+  </si>
+  <si>
+    <t>1.19.1A</t>
+  </si>
+  <si>
+    <t>1.19.1B</t>
   </si>
 </sst>
 </file>
@@ -1302,17 +1380,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1403,6 +1470,17 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1455,8 +1533,8 @@
       <xdr:rowOff>3206</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="538032" cy="174663"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CaixaDeTexto 1">
@@ -1544,7 +1622,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CaixaDeTexto 1">
@@ -1633,8 +1711,8 @@
       <xdr:rowOff>18446</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="462947" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CaixaDeTexto 2">
@@ -1725,7 +1803,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CaixaDeTexto 2">
@@ -1816,8 +1894,8 @@
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="437236" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CaixaDeTexto 3">
@@ -1905,7 +1983,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CaixaDeTexto 3">
@@ -1982,8 +2060,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="437236" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CaixaDeTexto 4">
@@ -2071,7 +2149,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CaixaDeTexto 4">
@@ -2148,8 +2226,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="437236" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CaixaDeTexto 6">
@@ -2237,7 +2315,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CaixaDeTexto 6">
@@ -2314,8 +2392,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="538032" cy="174663"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CaixaDeTexto 7">
@@ -2403,7 +2481,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CaixaDeTexto 7">
@@ -2492,8 +2570,8 @@
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="462947" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CaixaDeTexto 8">
@@ -2584,7 +2662,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CaixaDeTexto 8">
@@ -2675,8 +2753,8 @@
       <xdr:rowOff>26066</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="538032" cy="174663"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CaixaDeTexto 10">
@@ -2764,7 +2842,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CaixaDeTexto 10">
@@ -2853,8 +2931,8 @@
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="538032" cy="174663"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CaixaDeTexto 11">
@@ -2942,7 +3020,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CaixaDeTexto 11">
@@ -3031,8 +3109,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="538032" cy="174663"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="CaixaDeTexto 12">
@@ -3120,7 +3198,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="CaixaDeTexto 12">
@@ -3241,44 +3319,44 @@
     <tableColumn id="1" name="ID" dataDxfId="33"/>
     <tableColumn id="2" name="VLAN" dataDxfId="32"/>
     <tableColumn id="3" name="Nome vlan" dataDxfId="31"/>
-    <tableColumn id="4" name="Nº de Equipamentos a Endereçar" dataDxfId="2"/>
-    <tableColumn id="5" name="BASE 2" dataDxfId="1"/>
-    <tableColumn id="6" name="Prefix Network" dataDxfId="0"/>
+    <tableColumn id="4" name="Nº de Equipamentos a Endereçar" dataDxfId="30"/>
+    <tableColumn id="5" name="BASE 2" dataDxfId="29"/>
+    <tableColumn id="6" name="Prefix Network" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabela811" displayName="Tabela811" ref="A15:I25" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabela811" displayName="Tabela811" ref="A15:I25" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A15:I25"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="VLAN" dataDxfId="28"/>
-    <tableColumn id="2" name="Endereço de Rede" dataDxfId="27"/>
-    <tableColumn id="3" name="Máscara" dataDxfId="26"/>
-    <tableColumn id="4" name="Host Minínimo / _x000a_default gateway" dataDxfId="25"/>
-    <tableColumn id="5" name="Host Máximo" dataDxfId="24"/>
-    <tableColumn id="6" name="Endereço de Broadcast" dataDxfId="23"/>
-    <tableColumn id="7" name="Bits usados" dataDxfId="22"/>
-    <tableColumn id="8" name="Endereço Min. (binário)" dataDxfId="21"/>
-    <tableColumn id="9" name="Endereço Max. (binário)" dataDxfId="20"/>
+    <tableColumn id="1" name="VLAN" dataDxfId="25"/>
+    <tableColumn id="2" name="Endereço de Rede" dataDxfId="24"/>
+    <tableColumn id="3" name="Máscara" dataDxfId="23"/>
+    <tableColumn id="4" name="Host Minínimo / _x000a_default gateway" dataDxfId="22"/>
+    <tableColumn id="5" name="Host Máximo" dataDxfId="21"/>
+    <tableColumn id="6" name="Endereço de Broadcast" dataDxfId="20"/>
+    <tableColumn id="7" name="Bits usados" dataDxfId="19"/>
+    <tableColumn id="8" name="Endereço Min. (binário)" dataDxfId="18"/>
+    <tableColumn id="9" name="Endereço Max. (binário)" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="A3:H12" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="A3:H12" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A3:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Descrição da VLAN" dataDxfId="18"/>
-    <tableColumn id="2" name="Nome da VLAN" dataDxfId="17"/>
-    <tableColumn id="3" name="VLAN ID" dataDxfId="16"/>
-    <tableColumn id="4" name="Salas" dataDxfId="15"/>
-    <tableColumn id="5" name="Número de PC's" dataDxfId="14"/>
-    <tableColumn id="6" name="Número de outros equipamentos" dataDxfId="13"/>
-    <tableColumn id="7" name="Número total com folga" dataDxfId="12"/>
-    <tableColumn id="8" name="Endereço de rede" dataDxfId="11"/>
+    <tableColumn id="1" name="Descrição da VLAN" dataDxfId="15"/>
+    <tableColumn id="2" name="Nome da VLAN" dataDxfId="14"/>
+    <tableColumn id="3" name="VLAN ID" dataDxfId="13"/>
+    <tableColumn id="4" name="Salas" dataDxfId="12"/>
+    <tableColumn id="5" name="Número de PC's" dataDxfId="11"/>
+    <tableColumn id="6" name="Número de outros equipamentos" dataDxfId="10"/>
+    <tableColumn id="7" name="Número total com folga" dataDxfId="9"/>
+    <tableColumn id="8" name="Endereço de rede" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3296,16 +3374,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="A3:G135" totalsRowShown="0" dataDxfId="10">
-  <autoFilter ref="A3:G135"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="A3:G157" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A3:G157"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Sala" dataDxfId="9"/>
-    <tableColumn id="2" name="Tomada" dataDxfId="8"/>
-    <tableColumn id="3" name="Patch Panel" dataDxfId="7"/>
-    <tableColumn id="4" name="Switch" dataDxfId="6"/>
-    <tableColumn id="5" name="Porta" dataDxfId="5"/>
-    <tableColumn id="6" name="Tipo de Cabo" dataDxfId="4"/>
-    <tableColumn id="7" name="Em Utilização" dataDxfId="3"/>
+    <tableColumn id="1" name="Sala" dataDxfId="6"/>
+    <tableColumn id="2" name="Tomada" dataDxfId="5"/>
+    <tableColumn id="3" name="Patch Panel" dataDxfId="4"/>
+    <tableColumn id="4" name="Switch" dataDxfId="3"/>
+    <tableColumn id="5" name="Porta" dataDxfId="2"/>
+    <tableColumn id="6" name="Tipo de Cabo" dataDxfId="1"/>
+    <tableColumn id="7" name="Em Utilização" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3352,7 +3430,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3650,28 +3728,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3691,7 +3769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -3713,7 +3791,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -3735,7 +3813,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -3757,7 +3835,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -3779,7 +3857,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -3801,7 +3879,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -3823,7 +3901,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -3845,7 +3923,7 @@
       </c>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -3867,7 +3945,7 @@
       </c>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -3889,7 +3967,7 @@
       </c>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -3911,7 +3989,7 @@
       </c>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -3933,7 +4011,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -3955,7 +4033,7 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -3977,7 +4055,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -3999,7 +4077,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -4021,7 +4099,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -4032,7 +4110,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
@@ -4043,7 +4121,7 @@
       </c>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -4065,7 +4143,7 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -4087,7 +4165,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -4108,7 +4186,7 @@
       </c>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -4129,7 +4207,7 @@
       </c>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -4151,24 +4229,24 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4186,88 +4264,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" t="s">
         <v>268</v>
       </c>
-      <c r="B1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>99</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D2" s="16">
         <v>8</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>10</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D3" s="16">
         <v>22</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="20" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>20</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>69</v>
@@ -4277,46 +4355,46 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>30</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D5" s="16">
         <v>5</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>40</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D6" s="16">
         <v>3</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="20" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>50</v>
       </c>
@@ -4331,10 +4409,10 @@
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="20" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>60</v>
       </c>
@@ -4342,35 +4420,35 @@
         <v>78</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D8" s="16">
         <v>6</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>70</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D9" s="16">
         <v>10</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>80</v>
       </c>
@@ -4385,306 +4463,306 @@
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="20" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>90</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D11" s="16">
         <v>44</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="20" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="I15" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="G15" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>90</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C16" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="G16" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="H16" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>289</v>
-      </c>
       <c r="I16" s="12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>10</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="G17" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="H17" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="I17" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>99</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>20</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>30</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>60</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>344</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>347</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>70</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>348</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>351</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>40</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>352</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>355</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>50</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>356</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>359</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>80</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>360</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>363</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -4695,7 +4773,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -4706,7 +4784,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -4717,7 +4795,7 @@
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -4728,7 +4806,7 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -4739,22 +4817,22 @@
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>303</v>
+      </c>
+      <c r="C31" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>305</v>
-      </c>
-      <c r="C31" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -4776,29 +4854,29 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B1" s="21"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -4821,7 +4899,7 @@
         <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K3" t="s">
         <v>55</v>
@@ -4830,7 +4908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>56</v>
       </c>
@@ -4860,7 +4938,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -4890,7 +4968,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>67</v>
       </c>
@@ -4914,7 +4992,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -4938,7 +5016,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
@@ -4962,7 +5040,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -4986,7 +5064,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
@@ -5010,7 +5088,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>78</v>
       </c>
@@ -5034,7 +5112,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -5058,57 +5136,57 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -5125,36 +5203,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:P157"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5186,7 +5264,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>93</v>
       </c>
@@ -5215,7 +5293,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>93</v>
       </c>
@@ -5244,7 +5322,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>93</v>
       </c>
@@ -5273,7 +5351,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>93</v>
       </c>
@@ -5305,7 +5383,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>93</v>
       </c>
@@ -5326,7 +5404,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>93</v>
       </c>
@@ -5341,7 +5419,7 @@
         <v>106</v>
       </c>
       <c r="I9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L9" t="s">
         <v>88</v>
@@ -5350,7 +5428,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>93</v>
       </c>
@@ -5371,7 +5449,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>93</v>
       </c>
@@ -5395,7 +5473,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>119</v>
       </c>
@@ -5418,7 +5496,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>119</v>
       </c>
@@ -5441,7 +5519,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>119</v>
       </c>
@@ -5464,7 +5542,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>119</v>
       </c>
@@ -5487,7 +5565,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>119</v>
       </c>
@@ -5505,7 +5583,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>119</v>
       </c>
@@ -5526,7 +5604,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>119</v>
       </c>
@@ -5542,7 +5620,7 @@
       </c>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>119</v>
       </c>
@@ -5557,7 +5635,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>131</v>
       </c>
@@ -5580,7 +5658,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>131</v>
       </c>
@@ -5603,7 +5681,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>131</v>
       </c>
@@ -5626,7 +5704,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>131</v>
       </c>
@@ -5649,19 +5727,19 @@
         <v>103</v>
       </c>
       <c r="M23" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="N23" t="s">
         <v>87</v>
       </c>
       <c r="O23" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="P23" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>131</v>
       </c>
@@ -5676,7 +5754,7 @@
         <v>106</v>
       </c>
       <c r="M24" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -5688,7 +5766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>131</v>
       </c>
@@ -5703,19 +5781,19 @@
         <v>106</v>
       </c>
       <c r="M25" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="N25">
         <v>1</v>
       </c>
       <c r="O25" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="P25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>131</v>
       </c>
@@ -5742,7 +5820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>131</v>
       </c>
@@ -5757,7 +5835,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>140</v>
       </c>
@@ -5780,7 +5858,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>140</v>
       </c>
@@ -5803,7 +5881,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>140</v>
       </c>
@@ -5826,7 +5904,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>140</v>
       </c>
@@ -5849,7 +5927,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>140</v>
       </c>
@@ -5864,7 +5942,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>140</v>
       </c>
@@ -5879,7 +5957,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>140</v>
       </c>
@@ -5894,7 +5972,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>140</v>
       </c>
@@ -5909,7 +5987,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>149</v>
       </c>
@@ -5932,7 +6010,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>149</v>
       </c>
@@ -5955,10 +6033,10 @@
         <v>103</v>
       </c>
       <c r="H37" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>149</v>
       </c>
@@ -5973,7 +6051,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>149</v>
       </c>
@@ -5988,7 +6066,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>154</v>
       </c>
@@ -6011,7 +6089,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>154</v>
       </c>
@@ -6034,7 +6112,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>154</v>
       </c>
@@ -6057,7 +6135,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>154</v>
       </c>
@@ -6080,7 +6158,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>154</v>
       </c>
@@ -6095,7 +6173,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>154</v>
       </c>
@@ -6110,7 +6188,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>154</v>
       </c>
@@ -6125,7 +6203,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>154</v>
       </c>
@@ -6140,7 +6218,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>164</v>
       </c>
@@ -6163,7 +6241,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>164</v>
       </c>
@@ -6186,7 +6264,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>164</v>
       </c>
@@ -6209,7 +6287,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>164</v>
       </c>
@@ -6232,7 +6310,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>164</v>
       </c>
@@ -6255,7 +6333,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>164</v>
       </c>
@@ -6278,7 +6356,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>164</v>
       </c>
@@ -6293,7 +6371,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>164</v>
       </c>
@@ -6308,12 +6386,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>1.7</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -6323,12 +6401,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>1.7</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -6338,7 +6416,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>173</v>
       </c>
@@ -6361,7 +6439,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>173</v>
       </c>
@@ -6384,7 +6462,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>173</v>
       </c>
@@ -6407,7 +6485,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>173</v>
       </c>
@@ -6430,7 +6508,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>173</v>
       </c>
@@ -6445,7 +6523,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>173</v>
       </c>
@@ -6460,7 +6538,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>173</v>
       </c>
@@ -6475,7 +6553,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>173</v>
       </c>
@@ -6490,7 +6568,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>182</v>
       </c>
@@ -6513,7 +6591,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>182</v>
       </c>
@@ -6536,7 +6614,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>182</v>
       </c>
@@ -6559,7 +6637,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="19">
         <v>1.9</v>
       </c>
@@ -6582,15 +6660,15 @@
         <v>103</v>
       </c>
       <c r="H69" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>1.9</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -6600,12 +6678,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>1.9</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -6615,12 +6693,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>1.9</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -6630,12 +6708,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>1.9</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -6645,7 +6723,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>187</v>
       </c>
@@ -6656,7 +6734,7 @@
         <v>95</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E74" s="3">
         <v>3</v>
@@ -6668,7 +6746,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>187</v>
       </c>
@@ -6679,7 +6757,7 @@
         <v>95</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E75" s="3">
         <v>4</v>
@@ -6691,7 +6769,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>187</v>
       </c>
@@ -6702,7 +6780,7 @@
         <v>95</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E76" s="18">
         <v>5</v>
@@ -6714,7 +6792,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>187</v>
       </c>
@@ -6725,7 +6803,7 @@
         <v>95</v>
       </c>
       <c r="D77" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E77" s="19">
         <v>6</v>
@@ -6737,12 +6815,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -6752,12 +6830,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -6767,12 +6845,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -6782,12 +6860,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -6797,7 +6875,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>191</v>
       </c>
@@ -6808,7 +6886,7 @@
         <v>95</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E82" s="3">
         <v>5</v>
@@ -6820,7 +6898,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>191</v>
       </c>
@@ -6831,7 +6909,7 @@
         <v>95</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E83" s="3">
         <v>6</v>
@@ -6843,7 +6921,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>191</v>
       </c>
@@ -6854,7 +6932,7 @@
         <v>95</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E84" s="3">
         <v>7</v>
@@ -6866,7 +6944,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>191</v>
       </c>
@@ -6877,7 +6955,7 @@
         <v>95</v>
       </c>
       <c r="D85" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E85" s="19">
         <v>8</v>
@@ -6889,7 +6967,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>191</v>
       </c>
@@ -6904,7 +6982,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>191</v>
       </c>
@@ -6919,7 +6997,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>191</v>
       </c>
@@ -6934,7 +7012,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>191</v>
       </c>
@@ -6949,7 +7027,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>200</v>
       </c>
@@ -6960,7 +7038,7 @@
         <v>95</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E90" s="3">
         <v>9</v>
@@ -6972,7 +7050,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>200</v>
       </c>
@@ -6983,7 +7061,7 @@
         <v>95</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E91" s="3">
         <v>10</v>
@@ -6995,7 +7073,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
         <v>200</v>
       </c>
@@ -7006,7 +7084,7 @@
         <v>95</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E92" s="18">
         <v>11</v>
@@ -7018,7 +7096,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="19">
         <v>1.1200000000000001</v>
       </c>
@@ -7029,7 +7107,7 @@
         <v>95</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E93" s="19">
         <v>12</v>
@@ -7040,16 +7118,13 @@
       <c r="G93" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H93" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>1.1200000000000001</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -7059,12 +7134,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>1.1200000000000001</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -7074,12 +7149,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>1.1200000000000001</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -7089,12 +7164,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>1.1200000000000001</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -7104,7 +7179,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>205</v>
       </c>
@@ -7115,10 +7190,10 @@
         <v>95</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>156</v>
+        <v>314</v>
       </c>
       <c r="E98" s="3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F98" s="3" t="s">
         <v>97</v>
@@ -7127,7 +7202,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>205</v>
       </c>
@@ -7138,19 +7213,19 @@
         <v>95</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>156</v>
+        <v>314</v>
       </c>
       <c r="E99" s="3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>97</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>205</v>
       </c>
@@ -7161,10 +7236,10 @@
         <v>95</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>156</v>
+        <v>314</v>
       </c>
       <c r="E100" s="3">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>97</v>
@@ -7173,7 +7248,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>205</v>
       </c>
@@ -7184,10 +7259,10 @@
         <v>95</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>156</v>
+        <v>314</v>
       </c>
       <c r="E101" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>97</v>
@@ -7196,127 +7271,143 @@
         <v>103</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="5" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5" t="s">
+      <c r="C102" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="E102" s="18">
+        <v>17</v>
+      </c>
+      <c r="F102" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G102" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B103" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="C103" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D103" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="E103" s="19">
+        <v>18</v>
+      </c>
+      <c r="F103" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G103" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="E104" s="18">
+        <v>19</v>
+      </c>
+      <c r="F104" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G104" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="C105" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D105" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="E105" s="19">
+        <v>20</v>
+      </c>
+      <c r="F105" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G105" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5" t="s">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B105" s="5" t="s">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B106" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E106" s="3">
-        <v>13</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E107" s="3">
-        <v>14</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>217</v>
-      </c>
       <c r="C108" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>156</v>
+        <v>378</v>
       </c>
       <c r="E108" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>97</v>
@@ -7324,274 +7415,313 @@
       <c r="G108" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H108" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B109" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E109" s="3">
+        <v>4</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E110" s="3">
+        <v>5</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E111" s="3">
+        <v>6</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E109" s="3">
-        <v>16</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G109" s="3" t="s">
+      <c r="C112" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E112" s="3">
+        <v>7</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G112" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B110" s="3" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B113" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E110" s="3">
-        <v>17</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G110" s="3" t="s">
+      <c r="C113" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D113" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="E113" s="19">
+        <v>8</v>
+      </c>
+      <c r="F113" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G113" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B111" s="5" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B114" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
-      <c r="G111" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B112" s="5" t="s">
+      <c r="C114" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D114" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="E114" s="18">
+        <v>9</v>
+      </c>
+      <c r="F114" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G114" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B115" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E114" s="3">
-        <v>18</v>
-      </c>
-      <c r="F114" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E115" s="3">
-        <v>19</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G115" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E116" s="3">
-        <v>20</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G116" s="3" t="s">
+      <c r="C115" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D115" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="E115" s="19">
+        <v>10</v>
+      </c>
+      <c r="F115" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G115" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H116" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="5" t="s">
-        <v>223</v>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <v>1.1399999999999999</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>227</v>
+        <v>377</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
       <c r="F117" s="5"/>
-      <c r="G117" s="5" t="s">
+      <c r="G117" s="5"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E118" s="3">
+        <v>11</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E119" s="3">
+        <v>12</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E120" s="3">
+        <v>13</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D121" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="E121" s="19">
+        <v>14</v>
+      </c>
+      <c r="F121" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G121" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="H121" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B118" s="5" t="s">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B123" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A121" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A122" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E122" s="3">
-        <v>24</v>
-      </c>
-      <c r="F122" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A123" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>234</v>
       </c>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -7601,223 +7731,684 @@
         <v>106</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="3" t="s">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="18">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B126" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="C126" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D126" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="E126" s="18">
+        <v>15</v>
+      </c>
+      <c r="F126" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G126" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="19">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B127" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="C127" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D127" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="E127" s="19">
+        <v>16</v>
+      </c>
+      <c r="F127" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G127" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="18">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B128" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="C128" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D128" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="E128" s="18">
+        <v>17</v>
+      </c>
+      <c r="F128" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G128" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="19">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B129" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="C129" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D129" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="E129" s="19">
+        <v>18</v>
+      </c>
+      <c r="F129" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G129" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E130" s="3">
+        <v>19</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="19">
+        <v>1.17</v>
+      </c>
+      <c r="B131" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C131" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D131" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="E131" s="19">
+        <v>20</v>
+      </c>
+      <c r="F131" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G131" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="18">
+        <v>1.17</v>
+      </c>
+      <c r="B132" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="C132" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D132" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="E132" s="18">
+        <v>3</v>
+      </c>
+      <c r="F132" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G132" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H132" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="19">
+        <v>1.17</v>
+      </c>
+      <c r="B133" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="C133" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D133" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="E133" s="19">
+        <v>4</v>
+      </c>
+      <c r="F133" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G133" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="18">
+        <v>1.17</v>
+      </c>
+      <c r="B134" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="C134" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D134" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="E134" s="18">
+        <v>5</v>
+      </c>
+      <c r="F134" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G134" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="19">
+        <v>1.17</v>
+      </c>
+      <c r="B135" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="C135" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D135" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="E135" s="19">
+        <v>6</v>
+      </c>
+      <c r="F135" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G135" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="18">
+        <v>1.17</v>
+      </c>
+      <c r="B136" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="C136" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D136" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="E136" s="18">
+        <v>7</v>
+      </c>
+      <c r="F136" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G136" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="19">
+        <v>1.17</v>
+      </c>
+      <c r="B137" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="C137" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D137" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="E137" s="19">
+        <v>8</v>
+      </c>
+      <c r="F137" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G137" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="18">
+        <v>1.17</v>
+      </c>
+      <c r="B138" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="C138" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D138" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="E138" s="18">
+        <v>9</v>
+      </c>
+      <c r="F138" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G138" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="19">
+        <v>1.17</v>
+      </c>
+      <c r="B139" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="C139" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D139" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="E139" s="19">
+        <v>10</v>
+      </c>
+      <c r="F139" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G139" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="5">
+        <v>1.17</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="5">
+        <v>1.17</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B142" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="C142" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E142" s="3">
+        <v>11</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E124" s="3">
-        <v>21</v>
-      </c>
-      <c r="F124" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G124" s="3" t="s">
+      <c r="C143" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E143" s="3">
+        <v>12</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B144" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D144" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="E144" s="18">
+        <v>13</v>
+      </c>
+      <c r="F144" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G144" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A125" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E125" s="3">
-        <v>22</v>
-      </c>
-      <c r="F125" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G125" s="3" t="s">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B145" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C145" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D145" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="E145" s="19">
+        <v>14</v>
+      </c>
+      <c r="F145" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G145" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="5" t="s">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="5">
+        <v>1.18</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="5">
+        <v>1.18</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+      <c r="G147" s="5"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="18">
+        <v>1.19</v>
+      </c>
+      <c r="B148" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D148" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="E148" s="18">
+        <v>15</v>
+      </c>
+      <c r="F148" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G148" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="5">
+        <v>1.19</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+      <c r="G149" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A127" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B127" s="5" t="s">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5"/>
-      <c r="E127" s="5"/>
-      <c r="F127" s="5"/>
-      <c r="G127" s="5" t="s">
+      <c r="B150" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E150" s="3">
+        <v>16</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E151" s="3">
+        <v>17</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="E152" s="9">
+        <v>18</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G152" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+      <c r="G153" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E128" s="3">
-        <v>23</v>
-      </c>
-      <c r="F128" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E129" s="3">
-        <v>24</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A130" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C130" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D130" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E130" s="9">
-        <v>25</v>
-      </c>
-      <c r="F130" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G130" s="9" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A131" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B131" s="5" t="s">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+      <c r="G154" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B155" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C131" s="5"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="5"/>
-      <c r="G131" s="5" t="s">
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
+      <c r="G155" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B132" s="5" t="s">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B156" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C132" s="5"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="5"/>
-      <c r="G132" s="5" t="s">
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+      <c r="G156" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B133" s="5" t="s">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B157" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="5"/>
-      <c r="G133" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B134" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C134" s="5"/>
-      <c r="D134" s="5"/>
-      <c r="E134" s="5"/>
-      <c r="F134" s="5"/>
-      <c r="G134" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C135" s="5"/>
-      <c r="D135" s="5"/>
-      <c r="E135" s="5"/>
-      <c r="F135" s="5"/>
-      <c r="G135" s="5" t="s">
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+      <c r="G157" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7845,24 +8436,24 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -7882,7 +8473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7896,7 +8487,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -7910,7 +8501,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>35</v>
       </c>
@@ -7921,7 +8512,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -7932,7 +8523,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -7946,7 +8537,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -7960,7 +8551,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>44</v>
       </c>
@@ -7971,7 +8562,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -8019,11 +8610,11 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>

</xml_diff>

<commit_message>
Tabelas alteradas com a sala certa
</commit_message>
<xml_diff>
--- a/Versão Final/Tabelas.xlsx
+++ b/Versão Final/Tabelas.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="402">
   <si>
     <t>Número Sala</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t>1.1.1A</t>
-  </si>
-  <si>
-    <t>Sala 1.16</t>
   </si>
   <si>
     <t>SW1.1</t>
@@ -1178,9 +1175,6 @@
     <t>MUDEI DE SWITCH</t>
   </si>
   <si>
-    <t>NÃO É SUPOSTO MUDARMOS A SALA DO BASTIDOR ? ESTA AQUI COMO SALA 1.16 MAS OS BASTIDORES ESTÃO NOUTRA SALA AGORA, E TEMOS DOIS BASTIDORES</t>
-  </si>
-  <si>
     <t>1.16.1A</t>
   </si>
   <si>
@@ -1239,6 +1233,12 @@
   </si>
   <si>
     <t>1.19.1B</t>
+  </si>
+  <si>
+    <t>Sala 1.21</t>
+  </si>
+  <si>
+    <t>Sala 1.20</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1363,6 +1363,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3743,11 +3746,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4110,7 +4113,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
@@ -4231,7 +4234,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4241,12 +4244,12 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4264,8 +4267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4283,22 +4286,22 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" t="s">
         <v>266</v>
       </c>
-      <c r="B1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>267</v>
-      </c>
-      <c r="F1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4306,20 +4309,20 @@
         <v>99</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D2" s="16">
         <v>8</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="G2" t="s">
         <v>271</v>
-      </c>
-      <c r="G2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4327,17 +4330,17 @@
         <v>10</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D3" s="16">
         <v>22</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4345,7 +4348,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>69</v>
@@ -4355,7 +4358,7 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4363,17 +4366,17 @@
         <v>30</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D5" s="16">
         <v>5</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4381,17 +4384,17 @@
         <v>40</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D6" s="16">
         <v>3</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4409,7 +4412,7 @@
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4420,14 +4423,14 @@
         <v>78</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D8" s="16">
         <v>6</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4435,17 +4438,17 @@
         <v>70</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D9" s="16">
         <v>10</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4463,7 +4466,7 @@
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4471,17 +4474,17 @@
         <v>90</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D11" s="16">
         <v>44</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4493,31 +4496,31 @@
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="G15" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="G15" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="H15" s="14" t="s">
+      <c r="I15" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4525,28 +4528,28 @@
         <v>90</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C16" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="H16" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="I16" s="12" t="s">
         <v>289</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -4554,28 +4557,28 @@
         <v>10</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="F17" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="G17" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="H17" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="I17" s="12" t="s">
         <v>295</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -4583,19 +4586,19 @@
         <v>99</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="E18" s="12" t="s">
+      <c r="F18" s="12" t="s">
         <v>333</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>334</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
@@ -4606,19 +4609,19 @@
         <v>20</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>336</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>337</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -4629,19 +4632,19 @@
         <v>30</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>339</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>340</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -4652,19 +4655,19 @@
         <v>60</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>343</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>344</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -4675,19 +4678,19 @@
         <v>70</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>347</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>348</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -4698,19 +4701,19 @@
         <v>40</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="F23" s="12" t="s">
         <v>351</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>352</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
@@ -4721,19 +4724,19 @@
         <v>50</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="F24" s="12" t="s">
         <v>355</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>356</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -4744,19 +4747,19 @@
         <v>80</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="F25" s="12" t="s">
         <v>359</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>360</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
@@ -4819,20 +4822,20 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -4850,7 +4853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -4871,10 +4874,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4899,7 +4902,7 @@
         <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K3" t="s">
         <v>55</v>
@@ -5138,7 +5141,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>83</v>
@@ -5146,47 +5149,47 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -5205,8 +5208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I149" sqref="I149"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5225,12 +5228,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="A1" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5272,25 +5275,25 @@
         <v>94</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="L4" t="s">
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -5298,28 +5301,28 @@
         <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s">
         <v>86</v>
       </c>
       <c r="M5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -5327,28 +5330,28 @@
         <v>93</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="E6" s="4">
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="L6" t="s">
         <v>40</v>
       </c>
       <c r="M6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -5356,31 +5359,31 @@
         <v>93</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="E7" s="19">
         <v>6</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L7" t="s">
         <v>33</v>
       </c>
       <c r="M7" t="s">
+        <v>106</v>
+      </c>
+      <c r="N7" t="s">
         <v>107</v>
-      </c>
-      <c r="N7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5388,20 +5391,20 @@
         <v>93</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L8" t="s">
         <v>87</v>
       </c>
       <c r="M8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5409,23 +5412,23 @@
         <v>93</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L9" t="s">
         <v>88</v>
       </c>
       <c r="M9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -5433,20 +5436,20 @@
         <v>93</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s">
+        <v>113</v>
+      </c>
+      <c r="M10" t="s">
         <v>114</v>
-      </c>
-      <c r="M10" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -5454,313 +5457,313 @@
         <v>93</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s">
         <v>30</v>
       </c>
       <c r="M11" t="s">
+        <v>116</v>
+      </c>
+      <c r="N11" t="s">
         <v>117</v>
-      </c>
-      <c r="N11" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E12" s="3">
         <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E13" s="3">
         <v>8</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="E14" s="7">
         <v>9</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="E15" s="19">
         <v>10</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L17" t="s">
         <v>127</v>
-      </c>
-      <c r="L17" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E20" s="3">
         <v>11</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E21" s="3">
         <v>12</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E22" s="3">
         <v>13</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="E23" s="19">
         <v>14</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="N23" t="s">
         <v>87</v>
       </c>
       <c r="O23" t="s">
+        <v>361</v>
+      </c>
+      <c r="P23" t="s">
         <v>362</v>
-      </c>
-      <c r="P23" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M24" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P24">
         <v>1</v>
@@ -5768,26 +5771,26 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N25">
         <v>1</v>
       </c>
       <c r="O25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="P25">
         <v>0</v>
@@ -5795,26 +5798,26 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N26">
         <v>2</v>
       </c>
       <c r="O26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -5822,568 +5825,568 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E28" s="3">
         <v>15</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C29" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E29" s="3">
         <v>16</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E30" s="3">
         <v>17</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D31" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="E31" s="19">
         <v>18</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E36" s="3">
         <v>19</v>
       </c>
       <c r="F36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C37" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="E37" s="19">
         <v>20</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H37" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="E40" s="3">
         <v>3</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>95</v>
+        <v>156</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E41" s="3">
         <v>4</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>95</v>
+        <v>157</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E42" s="3">
         <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E43" s="19">
         <v>6</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>95</v>
+      <c r="C48" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E48" s="3">
         <v>7</v>
       </c>
       <c r="F48" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>95</v>
+        <v>165</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E49" s="3">
         <v>8</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>95</v>
+        <v>166</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E50" s="3">
         <v>9</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E51" s="19">
         <v>10</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" s="18">
         <v>11</v>
       </c>
       <c r="F52" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G52" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E53" s="19">
         <v>12</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -6391,14 +6394,14 @@
         <v>1.7</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -6406,235 +6409,235 @@
         <v>1.7</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>95</v>
+      <c r="C58" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E58" s="3">
         <v>13</v>
       </c>
       <c r="F58" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>95</v>
+        <v>174</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E59" s="3">
         <v>14</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>95</v>
+        <v>175</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E60" s="3">
         <v>15</v>
       </c>
       <c r="F60" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>95</v>
+        <v>176</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E61" s="19">
         <v>16</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>95</v>
+      <c r="C66" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E66" s="3">
         <v>17</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>95</v>
+        <v>183</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E67" s="3">
         <v>18</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E68" s="18">
         <v>19</v>
       </c>
       <c r="F68" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G68" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G68" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -6642,25 +6645,25 @@
         <v>1.9</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E69" s="19">
         <v>20</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H69" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -6668,14 +6671,14 @@
         <v>1.9</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -6683,14 +6686,14 @@
         <v>1.9</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -6698,14 +6701,14 @@
         <v>1.9</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -6713,387 +6716,387 @@
         <v>1.9</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>95</v>
+      <c r="C74" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E74" s="3">
         <v>3</v>
       </c>
       <c r="F74" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>95</v>
+      <c r="C75" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E75" s="3">
         <v>4</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E76" s="18">
         <v>5</v>
       </c>
       <c r="F76" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G76" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G76" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D77" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E77" s="19">
         <v>6</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G77" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>95</v>
+      <c r="C82" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E82" s="3">
         <v>5</v>
       </c>
       <c r="F82" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G82" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>95</v>
+        <v>192</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E83" s="3">
         <v>6</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>95</v>
+        <v>193</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E84" s="3">
         <v>7</v>
       </c>
       <c r="F84" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G84" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D85" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E85" s="19">
         <v>8</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G85" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>95</v>
+      <c r="C90" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E90" s="3">
         <v>9</v>
       </c>
       <c r="F90" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G90" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>95</v>
+        <v>201</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E91" s="3">
         <v>10</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C92" s="18" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E92" s="18">
         <v>11</v>
       </c>
       <c r="F92" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G92" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G92" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -7101,22 +7104,22 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E93" s="19">
         <v>12</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G93" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -7124,14 +7127,14 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -7139,14 +7142,14 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -7154,14 +7157,14 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -7169,198 +7172,198 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B98" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>95</v>
+      <c r="C98" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E98" s="3">
         <v>13</v>
       </c>
       <c r="F98" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G98" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>95</v>
+        <v>206</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E99" s="3">
         <v>14</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>95</v>
+        <v>207</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E100" s="3">
         <v>15</v>
       </c>
       <c r="F100" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G100" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>95</v>
+        <v>208</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E101" s="3">
         <v>16</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E102" s="18">
         <v>17</v>
       </c>
       <c r="F102" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G102" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G102" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E103" s="19">
         <v>18</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G103" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E104" s="18">
         <v>19</v>
       </c>
       <c r="F104" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G104" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>95</v>
+        <v>400</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E105" s="19">
         <v>20</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G105" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -7368,14 +7371,14 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
       <c r="G106" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -7383,209 +7386,209 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
       <c r="G107" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B108" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>95</v>
+      <c r="C108" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E108" s="3">
         <v>3</v>
       </c>
       <c r="F108" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G108" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G108" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="H108" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>95</v>
+        <v>214</v>
+      </c>
+      <c r="C109" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E109" s="3">
         <v>4</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>95</v>
+        <v>215</v>
+      </c>
+      <c r="C110" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E110" s="3">
         <v>5</v>
       </c>
       <c r="F110" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G110" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>95</v>
+        <v>216</v>
+      </c>
+      <c r="C111" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E111" s="3">
         <v>6</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>95</v>
+        <v>217</v>
+      </c>
+      <c r="C112" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E112" s="3">
         <v>7</v>
       </c>
       <c r="F112" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G112" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G112" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D113" s="19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E113" s="19">
         <v>8</v>
       </c>
       <c r="F113" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G113" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C114" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E114" s="18">
         <v>9</v>
       </c>
       <c r="F114" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G114" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G114" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E115" s="19">
         <v>10</v>
       </c>
       <c r="F115" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G115" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>1.1399999999999999</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -7593,12 +7596,12 @@
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>1.1399999999999999</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -7606,228 +7609,225 @@
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B118" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>95</v>
+      <c r="C118" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E118" s="3">
         <v>11</v>
       </c>
       <c r="F118" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G118" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G118" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>95</v>
+        <v>223</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E119" s="3">
         <v>12</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>95</v>
+        <v>224</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E120" s="3">
         <v>13</v>
       </c>
       <c r="F120" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G120" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G120" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E121" s="19">
         <v>14</v>
       </c>
       <c r="F121" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G121" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H121" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
       <c r="G122" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
       <c r="G123" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
       <c r="G124" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
       <c r="G125" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="18">
         <v>1.1599999999999999</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C126" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E126" s="18">
         <v>15</v>
       </c>
       <c r="F126" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G126" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G126" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="19">
         <v>1.1599999999999999</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C127" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D127" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E127" s="19">
         <v>16</v>
       </c>
       <c r="F127" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G127" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="18">
         <v>1.1599999999999999</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C128" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E128" s="18">
         <v>17</v>
       </c>
       <c r="F128" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G128" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G128" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -7835,45 +7835,45 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="B129" s="19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D129" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E129" s="19">
         <v>18</v>
       </c>
       <c r="F129" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G129" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B130" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>95</v>
+      <c r="C130" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E130" s="3">
         <v>19</v>
       </c>
       <c r="F130" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G130" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G130" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -7881,22 +7881,22 @@
         <v>1.17</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D131" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E131" s="19">
         <v>20</v>
       </c>
       <c r="F131" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G131" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -7904,25 +7904,25 @@
         <v>1.17</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C132" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E132" s="18">
         <v>3</v>
       </c>
       <c r="F132" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G132" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G132" s="18" t="s">
-        <v>98</v>
-      </c>
       <c r="H132" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -7930,22 +7930,22 @@
         <v>1.17</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E133" s="19">
         <v>4</v>
       </c>
       <c r="F133" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G133" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -7953,22 +7953,22 @@
         <v>1.17</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C134" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E134" s="18">
         <v>5</v>
       </c>
       <c r="F134" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G134" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G134" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -7976,22 +7976,22 @@
         <v>1.17</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E135" s="19">
         <v>6</v>
       </c>
       <c r="F135" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G135" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -7999,22 +7999,22 @@
         <v>1.17</v>
       </c>
       <c r="B136" s="18" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C136" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E136" s="18">
         <v>7</v>
       </c>
       <c r="F136" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G136" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G136" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -8022,22 +8022,22 @@
         <v>1.17</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D137" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E137" s="19">
         <v>8</v>
       </c>
       <c r="F137" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G137" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -8045,22 +8045,22 @@
         <v>1.17</v>
       </c>
       <c r="B138" s="18" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C138" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D138" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E138" s="18">
         <v>9</v>
       </c>
       <c r="F138" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G138" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G138" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -8068,22 +8068,22 @@
         <v>1.17</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E139" s="19">
         <v>10</v>
       </c>
       <c r="F139" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G139" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -8091,7 +8091,7 @@
         <v>1.17</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -8104,7 +8104,7 @@
         <v>1.17</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -8114,94 +8114,94 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B142" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B142" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>95</v>
+      <c r="C142" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E142" s="3">
         <v>11</v>
       </c>
       <c r="F142" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G142" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="G142" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>95</v>
+        <v>235</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E143" s="3">
         <v>12</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C144" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D144" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E144" s="18">
         <v>13</v>
       </c>
       <c r="F144" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G144" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="G144" s="18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C145" s="19" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E145" s="19">
         <v>14</v>
       </c>
       <c r="F145" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G145" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -8209,7 +8209,7 @@
         <v>1.18</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -8222,7 +8222,7 @@
         <v>1.18</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
@@ -8235,22 +8235,22 @@
         <v>1.19</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C148" s="18" t="s">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="D148" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E148" s="18">
         <v>15</v>
       </c>
       <c r="F148" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G148" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -8258,158 +8258,158 @@
         <v>1.19</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
       <c r="G149" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B150" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B150" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>95</v>
+      <c r="C150" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E150" s="3">
         <v>16</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>95</v>
+        <v>241</v>
+      </c>
+      <c r="C151" s="21" t="s">
+        <v>401</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E151" s="3">
         <v>17</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="E152" s="9">
+      <c r="A152" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="D152" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="E152" s="18">
         <v>18</v>
       </c>
-      <c r="F152" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G152" s="9" t="s">
-        <v>241</v>
+      <c r="F152" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G152" s="18" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
       <c r="G153" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
       <c r="E154" s="5"/>
       <c r="F154" s="5"/>
       <c r="G154" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
       <c r="G155" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
       <c r="G156" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
       <c r="F157" s="5"/>
       <c r="G157" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -8447,11 +8447,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -8613,11 +8613,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="A1" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>